<commit_message>
Mise à jour des assets, pour le sprint 3
</commit_message>
<xml_diff>
--- a/documentation/Product-Backlog-Stampee.xlsx
+++ b/documentation/Product-Backlog-Stampee.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\stampee\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D724045-B5CD-4563-BA83-82B74E1D0F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661937DB-E8E0-4C26-9698-76AA29799E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <definedName name="Type" localSheetId="1">'[2]Maintenance Work Order'!#REF!</definedName>
     <definedName name="Type" localSheetId="0">'[2]Maintenance Work Order'!#REF!</definedName>
     <definedName name="Type">'[2]Maintenance Work Order'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Backlog Stampee'!$B$1:$J$94</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Backlog Stampee'!$B$1:$J$77</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'EXEMPLE Backlog produit'!$B$1:$I$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="254">
   <si>
     <t>TOTAL</t>
   </si>
@@ -802,6 +802,15 @@
   </si>
   <si>
     <t xml:space="preserve">Mise en avant de toutes les infos liées	</t>
+  </si>
+  <si>
+    <t>Guide Utilisateur</t>
+  </si>
+  <si>
+    <t>Expliquer le mode d'emploi de la plate forme</t>
+  </si>
+  <si>
+    <t>Facilité l'acces au utilisateurs et admins</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1107,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1204,6 +1213,30 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1225,29 +1258,26 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1825,30 +1855,30 @@
   <sheetData>
     <row r="1" spans="1:13" s="7" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
     </row>
     <row r="2" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="42"/>
+      <c r="D3" s="50"/>
       <c r="E3" s="13" t="s">
         <v>6</v>
       </c>
@@ -1875,10 +1905,10 @@
       <c r="B4" s="21">
         <v>123</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="10" t="s">
         <v>11</v>
       </c>
@@ -1905,10 +1935,10 @@
       <c r="B5" s="21">
         <v>345</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" s="47"/>
       <c r="E5" s="10" t="s">
         <v>17</v>
       </c>
@@ -1935,10 +1965,10 @@
       <c r="B6" s="21">
         <v>567</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="39"/>
+      <c r="D6" s="47"/>
       <c r="E6" s="10" t="s">
         <v>22</v>
       </c>
@@ -1965,10 +1995,10 @@
       <c r="B7" s="21">
         <v>789</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="39"/>
+      <c r="D7" s="47"/>
       <c r="E7" s="10" t="s">
         <v>26</v>
       </c>
@@ -1990,8 +2020,8 @@
     </row>
     <row r="8" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="21"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
       <c r="G8" s="20" t="s">
@@ -2009,8 +2039,8 @@
     </row>
     <row r="9" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
       <c r="E9" s="10"/>
       <c r="F9" s="11"/>
       <c r="G9" s="20" t="s">
@@ -2025,8 +2055,8 @@
     </row>
     <row r="10" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
       <c r="G10" s="20" t="s">
@@ -2041,8 +2071,8 @@
     </row>
     <row r="11" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
       <c r="G11" s="20" t="s">
@@ -2057,8 +2087,8 @@
     </row>
     <row r="12" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="21"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
       <c r="G12" s="20" t="s">
@@ -2073,8 +2103,8 @@
     </row>
     <row r="13" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
       <c r="G13" s="20" t="s">
@@ -2089,8 +2119,8 @@
     </row>
     <row r="14" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
       <c r="G14" s="20" t="s">
@@ -2105,8 +2135,8 @@
     </row>
     <row r="15" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
       <c r="G15" s="20" t="s">
@@ -2121,8 +2151,8 @@
     </row>
     <row r="16" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
       <c r="G16" s="20" t="s">
@@ -2137,8 +2167,8 @@
     </row>
     <row r="17" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
       <c r="E17" s="10"/>
       <c r="F17" s="11"/>
       <c r="G17" s="20" t="s">
@@ -2152,14 +2182,14 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="45"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
       <c r="H18" s="24">
         <f>SUM(H4:H17)</f>
         <v>7</v>
@@ -2269,10 +2299,10 @@
     <tabColor theme="3" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A65" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.8984375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,20 +2326,20 @@
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
     </row>
     <row r="2" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="3" spans="1:14" s="6" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -2906,7 +2936,7 @@
       <c r="H21" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="46">
+      <c r="I21" s="39">
         <v>1</v>
       </c>
       <c r="J21" s="20" t="s">
@@ -2935,7 +2965,7 @@
       <c r="H22" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="46">
+      <c r="I22" s="39">
         <v>1</v>
       </c>
       <c r="J22" s="20" t="s">
@@ -2964,7 +2994,7 @@
       <c r="H23" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="46">
+      <c r="I23" s="39">
         <v>1</v>
       </c>
       <c r="J23" s="20" t="s">
@@ -2993,7 +3023,7 @@
       <c r="H24" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="46">
+      <c r="I24" s="39">
         <v>1</v>
       </c>
       <c r="J24" s="20" t="s">
@@ -3022,7 +3052,7 @@
       <c r="H25" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I25" s="46">
+      <c r="I25" s="39">
         <v>1</v>
       </c>
       <c r="J25" s="20" t="s">
@@ -3051,7 +3081,7 @@
       <c r="H26" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="46">
+      <c r="I26" s="39">
         <v>1</v>
       </c>
       <c r="J26" s="20" t="s">
@@ -3080,7 +3110,7 @@
       <c r="H27" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I27" s="46">
+      <c r="I27" s="39">
         <v>1</v>
       </c>
       <c r="J27" s="20" t="s">
@@ -3109,7 +3139,7 @@
       <c r="H28" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I28" s="46">
+      <c r="I28" s="39">
         <v>1</v>
       </c>
       <c r="J28" s="20" t="s">
@@ -3138,7 +3168,7 @@
       <c r="H29" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I29" s="46">
+      <c r="I29" s="39">
         <v>1</v>
       </c>
       <c r="J29" s="20" t="s">
@@ -3167,7 +3197,7 @@
       <c r="H30" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I30" s="46">
+      <c r="I30" s="39">
         <v>1</v>
       </c>
       <c r="J30" s="20" t="s">
@@ -3196,7 +3226,7 @@
       <c r="H31" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I31" s="46">
+      <c r="I31" s="39">
         <v>1</v>
       </c>
       <c r="J31" s="20" t="s">
@@ -3225,11 +3255,11 @@
       <c r="H32" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I32" s="46">
+      <c r="I32" s="39">
         <v>1</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3254,7 +3284,7 @@
       <c r="H33" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="46">
+      <c r="I33" s="39">
         <v>1</v>
       </c>
       <c r="J33" s="20" t="s">
@@ -3283,7 +3313,7 @@
       <c r="H34" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I34" s="46">
+      <c r="I34" s="39">
         <v>1</v>
       </c>
       <c r="J34" s="20" t="s">
@@ -3312,7 +3342,7 @@
       <c r="H35" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I35" s="46">
+      <c r="I35" s="39">
         <v>1</v>
       </c>
       <c r="J35" s="20" t="s">
@@ -3341,7 +3371,7 @@
       <c r="H36" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I36" s="46">
+      <c r="I36" s="39">
         <v>1</v>
       </c>
       <c r="J36" s="20" t="s">
@@ -3370,7 +3400,7 @@
       <c r="H37" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="46">
+      <c r="I37" s="39">
         <v>1</v>
       </c>
       <c r="J37" s="20" t="s">
@@ -3399,7 +3429,7 @@
       <c r="H38" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I38" s="46">
+      <c r="I38" s="39">
         <v>1</v>
       </c>
       <c r="J38" s="20" t="s">
@@ -3428,7 +3458,7 @@
       <c r="H39" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="46">
+      <c r="I39" s="39">
         <v>1</v>
       </c>
       <c r="J39" s="20" t="s">
@@ -3457,7 +3487,7 @@
       <c r="H40" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="46">
+      <c r="I40" s="39">
         <v>1</v>
       </c>
       <c r="J40" s="20" t="s">
@@ -3486,7 +3516,7 @@
       <c r="H41" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I41" s="46">
+      <c r="I41" s="39">
         <v>1</v>
       </c>
       <c r="J41" s="20" t="s">
@@ -3515,7 +3545,7 @@
       <c r="H42" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I42" s="46">
+      <c r="I42" s="39">
         <v>1</v>
       </c>
       <c r="J42" s="20" t="s">
@@ -3544,7 +3574,7 @@
       <c r="H43" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I43" s="46">
+      <c r="I43" s="39">
         <v>1</v>
       </c>
       <c r="J43" s="20" t="s">
@@ -3573,7 +3603,7 @@
       <c r="H44" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I44" s="46">
+      <c r="I44" s="39">
         <v>1</v>
       </c>
       <c r="J44" s="20" t="s">
@@ -3602,7 +3632,7 @@
       <c r="H45" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I45" s="46">
+      <c r="I45" s="39">
         <v>1</v>
       </c>
       <c r="J45" s="20" t="s">
@@ -3631,11 +3661,11 @@
       <c r="H46" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="47">
+      <c r="I46" s="40">
         <v>2</v>
       </c>
       <c r="J46" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="2:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3660,11 +3690,11 @@
       <c r="H47" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I47" s="47">
+      <c r="I47" s="40">
         <v>2</v>
       </c>
       <c r="J47" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3689,11 +3719,11 @@
       <c r="H48" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I48" s="47">
+      <c r="I48" s="40">
         <v>2</v>
       </c>
       <c r="J48" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3718,11 +3748,11 @@
       <c r="H49" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I49" s="47">
+      <c r="I49" s="40">
         <v>2</v>
       </c>
       <c r="J49" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3747,11 +3777,11 @@
       <c r="H50" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I50" s="47">
+      <c r="I50" s="40">
         <v>2</v>
       </c>
       <c r="J50" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3776,11 +3806,11 @@
       <c r="H51" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="47">
+      <c r="I51" s="40">
         <v>2</v>
       </c>
       <c r="J51" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3805,11 +3835,11 @@
       <c r="H52" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I52" s="47">
+      <c r="I52" s="40">
         <v>2</v>
       </c>
       <c r="J52" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3834,11 +3864,11 @@
       <c r="H53" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I53" s="47">
+      <c r="I53" s="40">
         <v>2</v>
       </c>
       <c r="J53" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3863,11 +3893,11 @@
       <c r="H54" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I54" s="47">
+      <c r="I54" s="40">
         <v>2</v>
       </c>
       <c r="J54" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -3892,11 +3922,11 @@
       <c r="H55" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="47">
+      <c r="I55" s="40">
         <v>2</v>
       </c>
       <c r="J55" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N55" s="3"/>
     </row>
@@ -3922,11 +3952,11 @@
       <c r="H56" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I56" s="47">
+      <c r="I56" s="40">
         <v>2</v>
       </c>
       <c r="J56" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -3951,16 +3981,16 @@
       <c r="H57" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I57" s="47">
+      <c r="I57" s="40">
         <v>2</v>
       </c>
       <c r="J57" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N57" s="3"/>
     </row>
     <row r="58" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="28">
+      <c r="B58" s="54">
         <v>55</v>
       </c>
       <c r="C58" s="29" t="s">
@@ -3981,281 +4011,281 @@
       <c r="H58" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I58" s="47">
+      <c r="I58" s="40">
         <v>2</v>
       </c>
       <c r="J58" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N58" s="3"/>
     </row>
     <row r="59" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="28">
+      <c r="B59" s="54">
         <v>56</v>
       </c>
-      <c r="C59" s="29" t="s">
+      <c r="C59" s="41" t="s">
         <v>201</v>
       </c>
-      <c r="D59" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E59" s="31" t="s">
+      <c r="D59" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="F59" s="32" t="s">
+      <c r="F59" s="44" t="s">
         <v>202</v>
       </c>
-      <c r="G59" s="33">
+      <c r="G59" s="45">
         <v>1</v>
       </c>
       <c r="H59" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I59" s="47">
-        <v>2</v>
+      <c r="I59" s="40">
+        <v>3</v>
       </c>
       <c r="J59" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N59" s="3"/>
     </row>
     <row r="60" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="28">
+      <c r="B60" s="54">
         <v>57</v>
       </c>
-      <c r="C60" s="29" t="s">
+      <c r="C60" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="D60" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E60" s="31" t="s">
+      <c r="D60" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="F60" s="32" t="s">
+      <c r="F60" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="G60" s="33">
+      <c r="G60" s="45">
         <v>2</v>
       </c>
       <c r="H60" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I60" s="47">
-        <v>2</v>
+      <c r="I60" s="40">
+        <v>3</v>
       </c>
       <c r="J60" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N60" s="3"/>
     </row>
     <row r="61" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="28">
+      <c r="B61" s="54">
         <v>58</v>
       </c>
-      <c r="C61" s="29" t="s">
+      <c r="C61" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="D61" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E61" s="31" t="s">
+      <c r="D61" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="F61" s="32" t="s">
+      <c r="F61" s="44" t="s">
         <v>174</v>
       </c>
-      <c r="G61" s="33">
+      <c r="G61" s="45">
         <v>1</v>
       </c>
       <c r="H61" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I61" s="47">
-        <v>2</v>
+      <c r="I61" s="40">
+        <v>3</v>
       </c>
       <c r="J61" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N61" s="3"/>
     </row>
     <row r="62" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="28">
+      <c r="B62" s="54">
         <v>59</v>
       </c>
-      <c r="C62" s="29" t="s">
+      <c r="C62" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="D62" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E62" s="31" t="s">
+      <c r="D62" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="F62" s="32" t="s">
+      <c r="F62" s="44" t="s">
         <v>209</v>
       </c>
-      <c r="G62" s="33">
+      <c r="G62" s="45">
         <v>2</v>
       </c>
       <c r="H62" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I62" s="47">
-        <v>2</v>
+      <c r="I62" s="40">
+        <v>3</v>
       </c>
       <c r="J62" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N62" s="3"/>
     </row>
     <row r="63" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="28">
+      <c r="B63" s="54">
         <v>60</v>
       </c>
-      <c r="C63" s="29" t="s">
+      <c r="C63" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="D63" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E63" s="31" t="s">
+      <c r="D63" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E63" s="43" t="s">
         <v>211</v>
       </c>
-      <c r="F63" s="32" t="s">
+      <c r="F63" s="44" t="s">
         <v>212</v>
       </c>
-      <c r="G63" s="33">
+      <c r="G63" s="45">
         <v>2</v>
       </c>
       <c r="H63" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I63" s="47">
-        <v>2</v>
+      <c r="I63" s="40">
+        <v>3</v>
       </c>
       <c r="J63" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N63" s="3"/>
     </row>
     <row r="64" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="28">
+      <c r="B64" s="54">
         <v>61</v>
       </c>
-      <c r="C64" s="29" t="s">
+      <c r="C64" s="41" t="s">
         <v>213</v>
       </c>
-      <c r="D64" s="30" t="s">
+      <c r="D64" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="E64" s="31" t="s">
+      <c r="E64" s="43" t="s">
         <v>214</v>
       </c>
-      <c r="F64" s="32" t="s">
+      <c r="F64" s="44" t="s">
         <v>216</v>
       </c>
-      <c r="G64" s="33">
+      <c r="G64" s="45">
         <v>1</v>
       </c>
       <c r="H64" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I64" s="47">
-        <v>2</v>
+      <c r="I64" s="40">
+        <v>3</v>
       </c>
       <c r="J64" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N64" s="3"/>
     </row>
     <row r="65" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="28">
+      <c r="B65" s="54">
         <v>62</v>
       </c>
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="41" t="s">
         <v>217</v>
       </c>
-      <c r="D65" s="30" t="s">
+      <c r="D65" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="E65" s="31" t="s">
+      <c r="E65" s="43" t="s">
         <v>218</v>
       </c>
-      <c r="F65" s="32" t="s">
+      <c r="F65" s="44" t="s">
         <v>219</v>
       </c>
-      <c r="G65" s="33">
+      <c r="G65" s="45">
         <v>1</v>
       </c>
       <c r="H65" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="I65" s="47">
-        <v>2</v>
+      <c r="I65" s="40">
+        <v>3</v>
       </c>
       <c r="J65" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N65" s="3"/>
     </row>
     <row r="66" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="28">
+      <c r="B66" s="54">
         <v>63</v>
       </c>
-      <c r="C66" s="29" t="s">
+      <c r="C66" s="41" t="s">
         <v>220</v>
       </c>
-      <c r="D66" s="30" t="s">
+      <c r="D66" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="E66" s="31" t="s">
+      <c r="E66" s="43" t="s">
         <v>221</v>
       </c>
-      <c r="F66" s="32" t="s">
+      <c r="F66" s="44" t="s">
         <v>222</v>
       </c>
-      <c r="G66" s="33">
+      <c r="G66" s="45">
         <v>1</v>
       </c>
       <c r="H66" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="I66" s="47">
-        <v>2</v>
+      <c r="I66" s="40">
+        <v>3</v>
       </c>
       <c r="J66" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N66" s="3"/>
     </row>
     <row r="67" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="28">
+      <c r="B67" s="54">
         <v>64</v>
       </c>
-      <c r="C67" s="29" t="s">
+      <c r="C67" s="41" t="s">
         <v>223</v>
       </c>
-      <c r="D67" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E67" s="31" t="s">
+      <c r="D67" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E67" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="F67" s="32" t="s">
+      <c r="F67" s="44" t="s">
         <v>225</v>
       </c>
-      <c r="G67" s="33">
+      <c r="G67" s="45">
         <v>1</v>
       </c>
       <c r="H67" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I67" s="47">
-        <v>2</v>
+      <c r="I67" s="40">
+        <v>3</v>
       </c>
       <c r="J67" s="20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N67" s="3"/>
     </row>
@@ -4263,29 +4293,29 @@
       <c r="B68" s="28">
         <v>65</v>
       </c>
-      <c r="C68" s="48" t="s">
+      <c r="C68" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="D68" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E68" s="50" t="s">
+      <c r="D68" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E68" s="43" t="s">
         <v>227</v>
       </c>
-      <c r="F68" s="51" t="s">
+      <c r="F68" s="44" t="s">
         <v>228</v>
       </c>
-      <c r="G68" s="52">
-        <v>1</v>
+      <c r="G68" s="45">
+        <v>2</v>
       </c>
       <c r="H68" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I68" s="53">
+      <c r="I68" s="46">
         <v>3</v>
       </c>
       <c r="J68" s="20" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N68" s="3"/>
     </row>
@@ -4293,29 +4323,29 @@
       <c r="B69" s="28">
         <v>66</v>
       </c>
-      <c r="C69" s="48" t="s">
+      <c r="C69" s="41" t="s">
         <v>229</v>
       </c>
-      <c r="D69" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E69" s="50" t="s">
+      <c r="D69" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E69" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="F69" s="51" t="s">
+      <c r="F69" s="44" t="s">
         <v>231</v>
       </c>
-      <c r="G69" s="52">
-        <v>1</v>
+      <c r="G69" s="45">
+        <v>2</v>
       </c>
       <c r="H69" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I69" s="53">
+      <c r="I69" s="46">
         <v>3</v>
       </c>
       <c r="J69" s="20" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N69" s="3"/>
     </row>
@@ -4323,29 +4353,29 @@
       <c r="B70" s="28">
         <v>67</v>
       </c>
-      <c r="C70" s="48" t="s">
+      <c r="C70" s="41" t="s">
         <v>232</v>
       </c>
-      <c r="D70" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E70" s="50" t="s">
+      <c r="D70" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E70" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="F70" s="51" t="s">
+      <c r="F70" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="G70" s="52">
-        <v>1</v>
+      <c r="G70" s="45">
+        <v>2</v>
       </c>
       <c r="H70" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I70" s="53">
+      <c r="I70" s="46">
         <v>3</v>
       </c>
       <c r="J70" s="20" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N70" s="3"/>
     </row>
@@ -4353,29 +4383,29 @@
       <c r="B71" s="28">
         <v>68</v>
       </c>
-      <c r="C71" s="48" t="s">
+      <c r="C71" s="41" t="s">
         <v>235</v>
       </c>
-      <c r="D71" s="49" t="s">
+      <c r="D71" s="42" t="s">
         <v>241</v>
       </c>
-      <c r="E71" s="50" t="s">
+      <c r="E71" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="F71" s="51" t="s">
+      <c r="F71" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="G71" s="52">
-        <v>1</v>
+      <c r="G71" s="45">
+        <v>2</v>
       </c>
       <c r="H71" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I71" s="53">
+      <c r="I71" s="46">
         <v>3</v>
       </c>
       <c r="J71" s="20" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N71" s="3"/>
     </row>
@@ -4383,29 +4413,29 @@
       <c r="B72" s="28">
         <v>69</v>
       </c>
-      <c r="C72" s="48" t="s">
+      <c r="C72" s="41" t="s">
         <v>238</v>
       </c>
-      <c r="D72" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E72" s="50" t="s">
+      <c r="D72" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E72" s="43" t="s">
         <v>239</v>
       </c>
-      <c r="F72" s="51" t="s">
+      <c r="F72" s="44" t="s">
         <v>240</v>
       </c>
-      <c r="G72" s="52">
-        <v>1</v>
+      <c r="G72" s="45">
+        <v>2</v>
       </c>
       <c r="H72" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I72" s="53">
+      <c r="I72" s="46">
         <v>3</v>
       </c>
       <c r="J72" s="20" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N72" s="3"/>
     </row>
@@ -4413,29 +4443,29 @@
       <c r="B73" s="28">
         <v>70</v>
       </c>
-      <c r="C73" s="48" t="s">
+      <c r="C73" s="41" t="s">
         <v>242</v>
       </c>
-      <c r="D73" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E73" s="50" t="s">
+      <c r="D73" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E73" s="43" t="s">
         <v>243</v>
       </c>
-      <c r="F73" s="51" t="s">
+      <c r="F73" s="44" t="s">
         <v>244</v>
       </c>
-      <c r="G73" s="52">
-        <v>1</v>
+      <c r="G73" s="45">
+        <v>2</v>
       </c>
       <c r="H73" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I73" s="53">
+      <c r="I73" s="46">
         <v>3</v>
       </c>
       <c r="J73" s="20" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N73" s="3"/>
     </row>
@@ -4443,29 +4473,29 @@
       <c r="B74" s="28">
         <v>71</v>
       </c>
-      <c r="C74" s="48" t="s">
+      <c r="C74" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="D74" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E74" s="50" t="s">
+      <c r="D74" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E74" s="43" t="s">
         <v>246</v>
       </c>
-      <c r="F74" s="51" t="s">
+      <c r="F74" s="44" t="s">
         <v>247</v>
       </c>
-      <c r="G74" s="52">
-        <v>1</v>
+      <c r="G74" s="45">
+        <v>2</v>
       </c>
       <c r="H74" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I74" s="53">
+      <c r="I74" s="46">
         <v>3</v>
       </c>
       <c r="J74" s="20" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N74" s="3"/>
     </row>
@@ -4473,487 +4503,83 @@
       <c r="B75" s="28">
         <v>72</v>
       </c>
-      <c r="C75" s="48" t="s">
+      <c r="C75" s="41" t="s">
         <v>248</v>
       </c>
-      <c r="D75" s="49" t="s">
+      <c r="D75" s="42" t="s">
         <v>241</v>
       </c>
-      <c r="E75" s="50" t="s">
+      <c r="E75" s="43" t="s">
         <v>249</v>
       </c>
-      <c r="F75" s="51" t="s">
+      <c r="F75" s="44" t="s">
         <v>250</v>
       </c>
-      <c r="G75" s="52">
-        <v>1</v>
+      <c r="G75" s="45">
+        <v>2</v>
       </c>
       <c r="H75" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I75" s="53">
+      <c r="I75" s="46">
         <v>3</v>
       </c>
       <c r="J75" s="20" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N75" s="3"/>
     </row>
     <row r="76" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="28">
-        <v>73</v>
-      </c>
-      <c r="C76" s="48"/>
-      <c r="D76" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E76" s="50"/>
-      <c r="F76" s="51"/>
-      <c r="G76" s="52">
-        <v>1</v>
-      </c>
-      <c r="H76" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I76" s="53">
+      <c r="B76" s="55"/>
+      <c r="C76" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="D76" s="42" t="s">
+        <v>241</v>
+      </c>
+      <c r="E76" s="57" t="s">
+        <v>252</v>
+      </c>
+      <c r="F76" s="58" t="s">
+        <v>253</v>
+      </c>
+      <c r="G76" s="59">
+        <v>1</v>
+      </c>
+      <c r="H76" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="I76" s="46">
         <v>3</v>
       </c>
-      <c r="J76" s="20" t="s">
-        <v>15</v>
+      <c r="J76" s="60" t="s">
+        <v>14</v>
       </c>
       <c r="N76" s="3"/>
     </row>
     <row r="77" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="28">
-        <v>74</v>
-      </c>
-      <c r="C77" s="48"/>
-      <c r="D77" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E77" s="50"/>
-      <c r="F77" s="51"/>
-      <c r="G77" s="52">
-        <v>1</v>
-      </c>
-      <c r="H77" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I77" s="53">
-        <v>3</v>
-      </c>
-      <c r="J77" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N77" s="3"/>
-    </row>
-    <row r="78" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="28">
-        <v>75</v>
-      </c>
-      <c r="C78" s="48"/>
-      <c r="D78" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E78" s="50"/>
-      <c r="F78" s="51"/>
-      <c r="G78" s="52">
-        <v>1</v>
-      </c>
-      <c r="H78" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I78" s="53">
-        <v>3</v>
-      </c>
-      <c r="J78" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N78" s="3"/>
-    </row>
-    <row r="79" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="28">
-        <v>76</v>
-      </c>
-      <c r="C79" s="48"/>
-      <c r="D79" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E79" s="50"/>
-      <c r="F79" s="51"/>
-      <c r="G79" s="52">
-        <v>1</v>
-      </c>
-      <c r="H79" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I79" s="53">
-        <v>3</v>
-      </c>
-      <c r="J79" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N79" s="3"/>
-    </row>
-    <row r="80" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="28">
-        <v>77</v>
-      </c>
-      <c r="C80" s="48"/>
-      <c r="D80" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E80" s="50"/>
-      <c r="F80" s="51"/>
-      <c r="G80" s="52">
-        <v>1</v>
-      </c>
-      <c r="H80" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I80" s="53">
-        <v>3</v>
-      </c>
-      <c r="J80" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N80" s="3"/>
-    </row>
-    <row r="81" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="28">
-        <v>78</v>
-      </c>
-      <c r="C81" s="48"/>
-      <c r="D81" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E81" s="50"/>
-      <c r="F81" s="51"/>
-      <c r="G81" s="52">
-        <v>1</v>
-      </c>
-      <c r="H81" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I81" s="53">
-        <v>3</v>
-      </c>
-      <c r="J81" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N81" s="3"/>
-    </row>
-    <row r="82" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="28">
-        <v>79</v>
-      </c>
-      <c r="C82" s="48"/>
-      <c r="D82" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E82" s="50"/>
-      <c r="F82" s="51"/>
-      <c r="G82" s="52">
-        <v>1</v>
-      </c>
-      <c r="H82" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I82" s="53">
-        <v>3</v>
-      </c>
-      <c r="J82" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N82" s="3"/>
-    </row>
-    <row r="83" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="28">
-        <v>80</v>
-      </c>
-      <c r="C83" s="48"/>
-      <c r="D83" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E83" s="50"/>
-      <c r="F83" s="51"/>
-      <c r="G83" s="52">
-        <v>1</v>
-      </c>
-      <c r="H83" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I83" s="53">
-        <v>3</v>
-      </c>
-      <c r="J83" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N83" s="3"/>
-    </row>
-    <row r="84" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="28">
-        <v>81</v>
-      </c>
-      <c r="C84" s="48"/>
-      <c r="D84" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E84" s="50"/>
-      <c r="F84" s="51"/>
-      <c r="G84" s="52">
-        <v>1</v>
-      </c>
-      <c r="H84" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I84" s="53">
-        <v>3</v>
-      </c>
-      <c r="J84" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N84" s="3"/>
-    </row>
-    <row r="85" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="28">
-        <v>82</v>
-      </c>
-      <c r="C85" s="48"/>
-      <c r="D85" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E85" s="50"/>
-      <c r="F85" s="51"/>
-      <c r="G85" s="52">
-        <v>1</v>
-      </c>
-      <c r="H85" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I85" s="53">
-        <v>3</v>
-      </c>
-      <c r="J85" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N85" s="3"/>
-    </row>
-    <row r="86" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="28">
-        <v>83</v>
-      </c>
-      <c r="C86" s="48"/>
-      <c r="D86" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E86" s="50"/>
-      <c r="F86" s="51"/>
-      <c r="G86" s="52">
-        <v>1</v>
-      </c>
-      <c r="H86" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I86" s="53">
-        <v>3</v>
-      </c>
-      <c r="J86" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N86" s="3"/>
-    </row>
-    <row r="87" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="28">
-        <v>84</v>
-      </c>
-      <c r="C87" s="48"/>
-      <c r="D87" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E87" s="50"/>
-      <c r="F87" s="51"/>
-      <c r="G87" s="52">
-        <v>1</v>
-      </c>
-      <c r="H87" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I87" s="53">
-        <v>3</v>
-      </c>
-      <c r="J87" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N87" s="3"/>
-    </row>
-    <row r="88" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="28">
-        <v>85</v>
-      </c>
-      <c r="C88" s="48"/>
-      <c r="D88" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E88" s="50"/>
-      <c r="F88" s="51"/>
-      <c r="G88" s="52">
-        <v>1</v>
-      </c>
-      <c r="H88" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I88" s="53">
-        <v>3</v>
-      </c>
-      <c r="J88" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N88" s="3"/>
-    </row>
-    <row r="89" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="28">
-        <v>86</v>
-      </c>
-      <c r="C89" s="48"/>
-      <c r="D89" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E89" s="50"/>
-      <c r="F89" s="51"/>
-      <c r="G89" s="52">
-        <v>1</v>
-      </c>
-      <c r="H89" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I89" s="53">
-        <v>3</v>
-      </c>
-      <c r="J89" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N89" s="3"/>
-    </row>
-    <row r="90" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="28">
-        <v>87</v>
-      </c>
-      <c r="C90" s="48"/>
-      <c r="D90" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E90" s="50"/>
-      <c r="F90" s="51"/>
-      <c r="G90" s="52">
-        <v>1</v>
-      </c>
-      <c r="H90" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I90" s="53">
-        <v>3</v>
-      </c>
-      <c r="J90" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N90" s="3"/>
-    </row>
-    <row r="91" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="28">
-        <v>88</v>
-      </c>
-      <c r="C91" s="48"/>
-      <c r="D91" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E91" s="50"/>
-      <c r="F91" s="51"/>
-      <c r="G91" s="52">
-        <v>1</v>
-      </c>
-      <c r="H91" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I91" s="53">
-        <v>3</v>
-      </c>
-      <c r="J91" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N91" s="3"/>
-    </row>
-    <row r="92" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="28">
-        <v>89</v>
-      </c>
-      <c r="C92" s="48"/>
-      <c r="D92" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E92" s="50"/>
-      <c r="F92" s="51"/>
-      <c r="G92" s="52">
-        <v>1</v>
-      </c>
-      <c r="H92" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I92" s="53">
-        <v>3</v>
-      </c>
-      <c r="J92" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N92" s="3"/>
-    </row>
-    <row r="93" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="28">
-        <v>90</v>
-      </c>
-      <c r="C93" s="48"/>
-      <c r="D93" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E93" s="50"/>
-      <c r="F93" s="51"/>
-      <c r="G93" s="52">
-        <v>1</v>
-      </c>
-      <c r="H93" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="I93" s="53">
-        <v>3</v>
-      </c>
-      <c r="J93" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N93" s="3"/>
-    </row>
-    <row r="94" spans="2:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="43" t="s">
+      <c r="B77" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C94" s="44"/>
-      <c r="D94" s="44"/>
-      <c r="E94" s="44"/>
-      <c r="F94" s="44"/>
-      <c r="G94" s="44"/>
-      <c r="H94" s="45"/>
-      <c r="I94" s="23">
-        <f ca="1">SUM(I94:I108)</f>
+      <c r="C77" s="52"/>
+      <c r="D77" s="52"/>
+      <c r="E77" s="52"/>
+      <c r="F77" s="52"/>
+      <c r="G77" s="52"/>
+      <c r="H77" s="53"/>
+      <c r="I77" s="23">
+        <f ca="1">SUM(I77:I91)</f>
         <v>0</v>
       </c>
-      <c r="J94" s="22"/>
+      <c r="J77" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B94:H94"/>
+    <mergeCell ref="B77:H77"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
   </mergeCells>
-  <conditionalFormatting sqref="L4:L8 J4:J93">
+  <conditionalFormatting sqref="L4:L8 J4:J76">
     <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="En retard">
       <formula>NOT(ISERROR(SEARCH("En retard",J4)))</formula>
     </cfRule>
@@ -4970,7 +4596,7 @@
       <formula>NOT(ISERROR(SEARCH("Non commencé",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N4:N6 H4:H93">
+  <conditionalFormatting sqref="N4:N6 H4:H76">
     <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Faible">
       <formula>NOT(ISERROR(SEARCH("Faible",H4)))</formula>
     </cfRule>
@@ -4982,10 +4608,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H93" xr:uid="{C9161828-3D0A-4354-8FF9-0588FF283786}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H76" xr:uid="{C9161828-3D0A-4354-8FF9-0588FF283786}">
       <formula1>$N$4:$N$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:J93" xr:uid="{27263ABE-4B1D-4BFC-B079-C0425B7FF5F8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:J76" xr:uid="{27263ABE-4B1D-4BFC-B079-C0425B7FF5F8}">
       <formula1>$L$4:$L$8</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>